<commit_message>
Se termina metodo Clasifica
</commit_message>
<xml_diff>
--- a/TRAND.xlsx
+++ b/TRAND.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Esteban\Documents\ITQ\AUTOMATAS\Lexico3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0B043625-55FA-483B-9C18-D42FA1562063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B69D7C-DFF6-44FF-9875-FC05DFD6DCB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D379225A-E6C0-4E76-AED8-B0DF9717D839}"/>
   </bookViews>
@@ -127,7 +127,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,6 +175,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -196,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -217,6 +226,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -533,279 +545,276 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4C0A738-8F4D-42C3-940D-F79CCF44DCAD}">
-  <dimension ref="A1:AA43"/>
+  <dimension ref="A1:AA44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
+      <c r="B1">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1">
+        <v>11</v>
+      </c>
+      <c r="N1">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1">
+        <v>18</v>
+      </c>
+      <c r="U1">
+        <v>19</v>
+      </c>
+      <c r="V1">
+        <v>20</v>
+      </c>
+      <c r="W1">
+        <v>21</v>
+      </c>
+      <c r="X1">
+        <v>22</v>
+      </c>
+      <c r="Y1">
+        <v>23</v>
+      </c>
+      <c r="Z1">
+        <v>24</v>
+      </c>
+      <c r="AA1">
         <v>25</v>
       </c>
-      <c r="T1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5">
-        <v>0</v>
-      </c>
-      <c r="C2" s="5">
-        <v>1</v>
-      </c>
-      <c r="D2" s="5">
-        <v>1</v>
-      </c>
-      <c r="E2" s="5">
-        <v>33</v>
-      </c>
-      <c r="F2" s="5">
-        <v>1</v>
-      </c>
-      <c r="G2" s="5">
-        <v>12</v>
-      </c>
-      <c r="H2" s="5">
-        <v>14</v>
-      </c>
-      <c r="I2" s="5">
-        <v>8</v>
-      </c>
-      <c r="J2" s="5">
-        <v>9</v>
-      </c>
-      <c r="K2" s="5">
-        <v>10</v>
-      </c>
-      <c r="L2" s="5">
-        <v>11</v>
-      </c>
-      <c r="M2" s="5">
-        <v>23</v>
-      </c>
-      <c r="N2" s="5">
-        <v>16</v>
-      </c>
-      <c r="O2" s="5">
-        <v>16</v>
-      </c>
-      <c r="P2" s="5">
-        <v>18</v>
-      </c>
-      <c r="Q2" s="5">
-        <v>20</v>
-      </c>
-      <c r="R2" s="5">
-        <v>21</v>
-      </c>
-      <c r="S2" s="5">
-        <v>26</v>
-      </c>
-      <c r="T2" s="5">
-        <v>25</v>
-      </c>
-      <c r="U2" s="5">
-        <v>27</v>
-      </c>
-      <c r="V2" s="5">
-        <v>29</v>
-      </c>
-      <c r="W2" s="5">
-        <v>32</v>
-      </c>
-      <c r="X2" s="5">
-        <v>34</v>
-      </c>
-      <c r="Y2" s="5">
-        <v>0</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA2" s="5">
-        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>26</v>
+        <v>0</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0</v>
       </c>
       <c r="C3" s="5">
         <v>1</v>
       </c>
       <c r="D3" s="5">
-        <v>1</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>26</v>
+        <v>2</v>
+      </c>
+      <c r="E3" s="8">
+        <v>33</v>
       </c>
       <c r="F3" s="5">
         <v>1</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="V3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="X3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y3" s="3" t="s">
-        <v>26</v>
+      <c r="G3" s="5">
+        <v>12</v>
+      </c>
+      <c r="H3" s="5">
+        <v>14</v>
+      </c>
+      <c r="I3" s="5">
+        <v>8</v>
+      </c>
+      <c r="J3" s="5">
+        <v>9</v>
+      </c>
+      <c r="K3" s="5">
+        <v>10</v>
+      </c>
+      <c r="L3" s="5">
+        <v>11</v>
+      </c>
+      <c r="M3" s="5">
+        <v>23</v>
+      </c>
+      <c r="N3" s="5">
+        <v>16</v>
+      </c>
+      <c r="O3" s="5">
+        <v>16</v>
+      </c>
+      <c r="P3" s="5">
+        <v>18</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>20</v>
+      </c>
+      <c r="R3" s="5">
+        <v>21</v>
+      </c>
+      <c r="S3" s="5">
+        <v>26</v>
+      </c>
+      <c r="T3" s="5">
+        <v>25</v>
+      </c>
+      <c r="U3" s="5">
+        <v>27</v>
+      </c>
+      <c r="V3" s="5">
+        <v>29</v>
+      </c>
+      <c r="W3" s="5">
+        <v>32</v>
+      </c>
+      <c r="X3" s="5">
+        <v>34</v>
+      </c>
+      <c r="Y3" s="5">
+        <v>0</v>
       </c>
       <c r="Z3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AA3" s="3" t="s">
-        <v>26</v>
+      <c r="AA3" s="5">
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>26</v>
+      <c r="C4" s="5">
+        <v>1</v>
       </c>
       <c r="D4" s="5">
-        <v>2</v>
-      </c>
-      <c r="E4" s="5">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="F4" s="5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>26</v>
@@ -873,256 +882,256 @@
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="5">
+        <v>2</v>
+      </c>
+      <c r="E5" s="5">
         <v>3</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="5">
-        <v>4</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="O5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="P5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="R5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="S5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="T5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="U5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="V5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="W5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="X5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA5" s="6" t="s">
-        <v>27</v>
+      <c r="F5" s="5">
+        <v>5</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="W5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA5" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>26</v>
+        <v>3</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="D6" s="5">
         <v>4</v>
       </c>
-      <c r="E6" s="5">
-        <v>5</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="S6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="T6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="U6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="V6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="W6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="X6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA6" s="3" t="s">
-        <v>26</v>
+      <c r="E6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="R6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="S6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="T6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="U6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="V6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="W6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="X6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA6" s="6" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="5">
+        <v>4</v>
+      </c>
+      <c r="E7" s="5">
         <v>5</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="5">
-        <v>7</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" s="5">
-        <v>6</v>
-      </c>
-      <c r="H7" s="5">
-        <v>6</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="M7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="N7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="O7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="P7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="R7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="S7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="T7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="U7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="V7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="W7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="X7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA7" s="6" t="s">
-        <v>27</v>
+      <c r="F7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="T7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="U7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="V7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="W7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="X7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA7" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>27</v>
@@ -1139,11 +1148,11 @@
       <c r="F8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>27</v>
+      <c r="G8" s="5">
+        <v>6</v>
+      </c>
+      <c r="H8" s="5">
+        <v>6</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>27</v>
@@ -1205,90 +1214,90 @@
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>26</v>
+        <v>6</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="D9" s="5">
         <v>7</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="P9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="S9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="T9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="U9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="V9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="W9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="X9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA9" s="3" t="s">
-        <v>26</v>
+      <c r="E9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="R9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="S9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="T9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="U9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="V9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="W9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="X9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA9" s="6" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>26</v>
@@ -1296,8 +1305,8 @@
       <c r="C10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>26</v>
+      <c r="D10" s="5">
+        <v>7</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>26</v>
@@ -1308,7 +1317,7 @@
       <c r="G10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="4" t="s">
         <v>26</v>
       </c>
       <c r="I10" s="3" t="s">
@@ -1371,7 +1380,7 @@
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>26</v>
@@ -1454,7 +1463,7 @@
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>26</v>
@@ -1537,7 +1546,7 @@
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>26</v>
@@ -1620,7 +1629,7 @@
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>26</v>
@@ -1637,8 +1646,8 @@
       <c r="F14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G14" s="5">
-        <v>13</v>
+      <c r="G14" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>26</v>
@@ -1655,8 +1664,8 @@
       <c r="L14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="M14" s="5">
-        <v>13</v>
+      <c r="M14" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="N14" s="3" t="s">
         <v>26</v>
@@ -1703,26 +1712,26 @@
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
+        <v>12</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="5">
         <v>13</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="H15" s="3" t="s">
         <v>26</v>
       </c>
@@ -1738,8 +1747,8 @@
       <c r="L15" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="M15" s="3" t="s">
-        <v>26</v>
+      <c r="M15" s="5">
+        <v>13</v>
       </c>
       <c r="N15" s="3" t="s">
         <v>26</v>
@@ -1786,7 +1795,7 @@
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>26</v>
@@ -1821,8 +1830,8 @@
       <c r="L16" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="M16" s="5">
-        <v>13</v>
+      <c r="M16" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="N16" s="3" t="s">
         <v>26</v>
@@ -1842,8 +1851,8 @@
       <c r="S16" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="T16" s="5">
-        <v>15</v>
+      <c r="T16" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="U16" s="3" t="s">
         <v>26</v>
@@ -1869,64 +1878,64 @@
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
+        <v>14</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M17" s="5">
+        <v>13</v>
+      </c>
+      <c r="N17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="S17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="T17" s="5">
         <v>15</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="L17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="N17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="P17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="S17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="T17" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="U17" s="3" t="s">
         <v>26</v>
@@ -1952,7 +1961,7 @@
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>26</v>
@@ -1987,8 +1996,8 @@
       <c r="L18" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="M18" s="5">
-        <v>17</v>
+      <c r="M18" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="N18" s="3" t="s">
         <v>26</v>
@@ -2035,43 +2044,43 @@
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
+        <v>16</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M19" s="5">
         <v>17</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="L19" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M19" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="N19" s="3" t="s">
         <v>26</v>
@@ -2118,7 +2127,7 @@
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>26</v>
@@ -2162,8 +2171,8 @@
       <c r="O20" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="P20" s="5">
-        <v>19</v>
+      <c r="P20" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="Q20" s="3" t="s">
         <v>26</v>
@@ -2201,52 +2210,52 @@
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
+        <v>18</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P21" s="5">
         <v>19</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K21" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="L21" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M21" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="N21" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O21" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="P21" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="Q21" s="3" t="s">
         <v>26</v>
@@ -2284,7 +2293,7 @@
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>26</v>
@@ -2331,8 +2340,8 @@
       <c r="P22" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="Q22" s="5">
-        <v>19</v>
+      <c r="Q22" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="R22" s="3" t="s">
         <v>26</v>
@@ -2349,7 +2358,7 @@
       <c r="V22" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="W22" s="4" t="s">
+      <c r="W22" s="3" t="s">
         <v>26</v>
       </c>
       <c r="X22" s="3" t="s">
@@ -2367,7 +2376,7 @@
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>26</v>
@@ -2402,8 +2411,8 @@
       <c r="L23" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="M23" s="3">
-        <v>22</v>
+      <c r="M23" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="N23" s="3" t="s">
         <v>26</v>
@@ -2414,8 +2423,8 @@
       <c r="P23" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="Q23" s="3" t="s">
-        <v>26</v>
+      <c r="Q23" s="5">
+        <v>19</v>
       </c>
       <c r="R23" s="3" t="s">
         <v>26</v>
@@ -2432,7 +2441,7 @@
       <c r="V23" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="W23" s="3" t="s">
+      <c r="W23" s="4" t="s">
         <v>26</v>
       </c>
       <c r="X23" s="3" t="s">
@@ -2450,43 +2459,43 @@
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
+        <v>21</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M24" s="3">
         <v>22</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J24" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K24" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="L24" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M24" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="N24" s="3" t="s">
         <v>26</v>
@@ -2533,7 +2542,7 @@
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>26</v>
@@ -2568,8 +2577,8 @@
       <c r="L25" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="M25" s="5">
-        <v>24</v>
+      <c r="M25" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="N25" s="3" t="s">
         <v>26</v>
@@ -2616,43 +2625,43 @@
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
+        <v>23</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M26" s="5">
         <v>24</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J26" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K26" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="L26" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M26" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="N26" s="3" t="s">
         <v>26</v>
@@ -2699,7 +2708,7 @@
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>26</v>
@@ -2734,8 +2743,8 @@
       <c r="L27" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="M27" s="5">
-        <v>24</v>
+      <c r="M27" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="N27" s="3" t="s">
         <v>26</v>
@@ -2782,7 +2791,7 @@
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>26</v>
@@ -2838,8 +2847,8 @@
       <c r="S28" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="T28" s="3">
-        <v>24</v>
+      <c r="T28" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="U28" s="3" t="s">
         <v>26</v>
@@ -2865,422 +2874,422 @@
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
-        <v>27</v>
-      </c>
-      <c r="B29" s="5">
-        <v>27</v>
-      </c>
-      <c r="C29" s="5">
-        <v>27</v>
-      </c>
-      <c r="D29" s="5">
-        <v>27</v>
-      </c>
-      <c r="E29" s="5">
-        <v>27</v>
-      </c>
-      <c r="F29" s="5">
-        <v>27</v>
-      </c>
-      <c r="G29" s="5">
-        <v>27</v>
-      </c>
-      <c r="H29" s="5">
-        <v>27</v>
-      </c>
-      <c r="I29" s="5">
-        <v>27</v>
-      </c>
-      <c r="J29" s="5">
-        <v>27</v>
-      </c>
-      <c r="K29" s="5">
-        <v>27</v>
-      </c>
-      <c r="L29" s="5">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="M29" s="5">
-        <v>27</v>
-      </c>
-      <c r="N29" s="5">
-        <v>27</v>
-      </c>
-      <c r="O29" s="5">
-        <v>27</v>
-      </c>
-      <c r="P29" s="5">
-        <v>27</v>
-      </c>
-      <c r="Q29" s="5">
-        <v>27</v>
-      </c>
-      <c r="R29" s="5">
-        <v>27</v>
-      </c>
-      <c r="S29" s="5">
-        <v>27</v>
-      </c>
-      <c r="T29" s="5">
-        <v>27</v>
-      </c>
-      <c r="U29" s="5">
-        <v>28</v>
-      </c>
-      <c r="V29" s="5">
-        <v>27</v>
-      </c>
-      <c r="W29" s="5">
-        <v>27</v>
-      </c>
-      <c r="X29" s="5">
-        <v>27</v>
-      </c>
-      <c r="Y29" s="5">
-        <v>27</v>
-      </c>
-      <c r="Z29" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA29" s="5">
-        <v>27</v>
+        <v>24</v>
+      </c>
+      <c r="N29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="S29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="T29" s="3">
+        <v>24</v>
+      </c>
+      <c r="U29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="V29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="W29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="X29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA29" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
+        <v>27</v>
+      </c>
+      <c r="B30" s="5">
+        <v>27</v>
+      </c>
+      <c r="C30" s="5">
+        <v>27</v>
+      </c>
+      <c r="D30" s="5">
+        <v>27</v>
+      </c>
+      <c r="E30" s="5">
+        <v>27</v>
+      </c>
+      <c r="F30" s="5">
+        <v>27</v>
+      </c>
+      <c r="G30" s="5">
+        <v>27</v>
+      </c>
+      <c r="H30" s="5">
+        <v>27</v>
+      </c>
+      <c r="I30" s="5">
+        <v>27</v>
+      </c>
+      <c r="J30" s="5">
+        <v>27</v>
+      </c>
+      <c r="K30" s="5">
+        <v>27</v>
+      </c>
+      <c r="L30" s="5">
+        <v>27</v>
+      </c>
+      <c r="M30" s="5">
+        <v>27</v>
+      </c>
+      <c r="N30" s="5">
+        <v>27</v>
+      </c>
+      <c r="O30" s="5">
+        <v>27</v>
+      </c>
+      <c r="P30" s="5">
+        <v>27</v>
+      </c>
+      <c r="Q30" s="5">
+        <v>27</v>
+      </c>
+      <c r="R30" s="5">
+        <v>27</v>
+      </c>
+      <c r="S30" s="5">
+        <v>27</v>
+      </c>
+      <c r="T30" s="5">
+        <v>27</v>
+      </c>
+      <c r="U30" s="5">
         <v>28</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I30" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J30" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K30" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="L30" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M30" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="N30" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O30" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="P30" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q30" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R30" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="S30" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="T30" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="U30" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="V30" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="W30" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="X30" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y30" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z30" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA30" s="3" t="s">
-        <v>26</v>
+      <c r="V30" s="5">
+        <v>27</v>
+      </c>
+      <c r="W30" s="5">
+        <v>27</v>
+      </c>
+      <c r="X30" s="5">
+        <v>27</v>
+      </c>
+      <c r="Y30" s="5">
+        <v>27</v>
+      </c>
+      <c r="Z30" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA30" s="5">
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
-        <v>29</v>
-      </c>
-      <c r="B31" s="5">
-        <v>30</v>
-      </c>
-      <c r="C31" s="5">
-        <v>30</v>
-      </c>
-      <c r="D31" s="5">
-        <v>30</v>
-      </c>
-      <c r="E31" s="5">
-        <v>30</v>
-      </c>
-      <c r="F31" s="5">
-        <v>30</v>
-      </c>
-      <c r="G31" s="5">
-        <v>30</v>
-      </c>
-      <c r="H31" s="5">
-        <v>30</v>
-      </c>
-      <c r="I31" s="5">
-        <v>30</v>
-      </c>
-      <c r="J31" s="5">
-        <v>30</v>
-      </c>
-      <c r="K31" s="5">
-        <v>30</v>
-      </c>
-      <c r="L31" s="5">
-        <v>30</v>
-      </c>
-      <c r="M31" s="5">
-        <v>30</v>
-      </c>
-      <c r="N31" s="5">
-        <v>30</v>
-      </c>
-      <c r="O31" s="5">
-        <v>30</v>
-      </c>
-      <c r="P31" s="5">
-        <v>30</v>
-      </c>
-      <c r="Q31" s="5">
-        <v>30</v>
-      </c>
-      <c r="R31" s="5">
-        <v>30</v>
-      </c>
-      <c r="S31" s="5">
-        <v>30</v>
-      </c>
-      <c r="T31" s="5">
-        <v>30</v>
-      </c>
-      <c r="U31" s="5">
-        <v>30</v>
-      </c>
-      <c r="V31" s="5">
-        <v>30</v>
-      </c>
-      <c r="W31" s="5">
-        <v>30</v>
-      </c>
-      <c r="X31" s="5">
-        <v>30</v>
-      </c>
-      <c r="Y31" s="5">
-        <v>30</v>
-      </c>
-      <c r="Z31" s="5">
-        <v>30</v>
-      </c>
-      <c r="AA31" s="5">
-        <v>30</v>
+        <v>28</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="S31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="T31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="U31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="V31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="W31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="X31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA31" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
+        <v>29</v>
+      </c>
+      <c r="B32" s="5">
         <v>30</v>
       </c>
-      <c r="B32" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G32" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="H32" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="I32" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="J32" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="K32" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L32" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="M32" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="N32" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="O32" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="P32" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q32" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="R32" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="S32" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="T32" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="U32" s="6" t="s">
-        <v>27</v>
+      <c r="C32" s="5">
+        <v>30</v>
+      </c>
+      <c r="D32" s="5">
+        <v>30</v>
+      </c>
+      <c r="E32" s="5">
+        <v>30</v>
+      </c>
+      <c r="F32" s="5">
+        <v>30</v>
+      </c>
+      <c r="G32" s="5">
+        <v>30</v>
+      </c>
+      <c r="H32" s="5">
+        <v>30</v>
+      </c>
+      <c r="I32" s="5">
+        <v>30</v>
+      </c>
+      <c r="J32" s="5">
+        <v>30</v>
+      </c>
+      <c r="K32" s="5">
+        <v>30</v>
+      </c>
+      <c r="L32" s="5">
+        <v>30</v>
+      </c>
+      <c r="M32" s="5">
+        <v>30</v>
+      </c>
+      <c r="N32" s="5">
+        <v>30</v>
+      </c>
+      <c r="O32" s="5">
+        <v>30</v>
+      </c>
+      <c r="P32" s="5">
+        <v>30</v>
+      </c>
+      <c r="Q32" s="5">
+        <v>30</v>
+      </c>
+      <c r="R32" s="5">
+        <v>30</v>
+      </c>
+      <c r="S32" s="5">
+        <v>30</v>
+      </c>
+      <c r="T32" s="5">
+        <v>30</v>
+      </c>
+      <c r="U32" s="5">
+        <v>30</v>
       </c>
       <c r="V32" s="5">
-        <v>31</v>
-      </c>
-      <c r="W32" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="X32" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y32" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z32" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA32" s="6" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="W32" s="5">
+        <v>30</v>
+      </c>
+      <c r="X32" s="5">
+        <v>30</v>
+      </c>
+      <c r="Y32" s="5">
+        <v>30</v>
+      </c>
+      <c r="Z32" s="5">
+        <v>30</v>
+      </c>
+      <c r="AA32" s="5">
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
+        <v>30</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K33" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="L33" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M33" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="N33" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="O33" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="P33" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q33" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="R33" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="S33" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="T33" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="U33" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="V33" s="5">
         <v>31</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I33" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J33" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K33" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="L33" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M33" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="N33" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O33" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="P33" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q33" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R33" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="S33" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="T33" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="U33" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="V33" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="W33" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="X33" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y33" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z33" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA33" s="3" t="s">
-        <v>26</v>
+      <c r="W33" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="X33" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y33" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z33" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA33" s="6" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="34" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>26</v>
@@ -3288,8 +3297,8 @@
       <c r="C34" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D34" s="5">
-        <v>32</v>
+      <c r="D34" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>26</v>
@@ -3363,7 +3372,7 @@
     </row>
     <row r="35" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>26</v>
@@ -3371,8 +3380,8 @@
       <c r="C35" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>26</v>
+      <c r="D35" s="5">
+        <v>32</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>26</v>
@@ -3446,7 +3455,7 @@
     </row>
     <row r="36" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>26</v>
@@ -3481,11 +3490,11 @@
       <c r="L36" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="M36" s="5">
-        <v>17</v>
-      </c>
-      <c r="N36" s="5">
-        <v>36</v>
+      <c r="M36" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N36" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="O36" s="3" t="s">
         <v>26</v>
@@ -3514,8 +3523,8 @@
       <c r="W36" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="X36" s="5">
-        <v>35</v>
+      <c r="X36" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="Y36" s="3" t="s">
         <v>26</v>
@@ -3529,173 +3538,173 @@
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
-        <v>35</v>
-      </c>
-      <c r="B37" s="5">
-        <v>35</v>
-      </c>
-      <c r="C37" s="5">
-        <v>35</v>
-      </c>
-      <c r="D37" s="5">
-        <v>35</v>
-      </c>
-      <c r="E37" s="5">
-        <v>35</v>
-      </c>
-      <c r="F37" s="5">
-        <v>35</v>
-      </c>
-      <c r="G37" s="5">
-        <v>35</v>
-      </c>
-      <c r="H37" s="5">
-        <v>35</v>
-      </c>
-      <c r="I37" s="5">
-        <v>35</v>
-      </c>
-      <c r="J37" s="5">
-        <v>35</v>
-      </c>
-      <c r="K37" s="5">
-        <v>35</v>
-      </c>
-      <c r="L37" s="5">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K37" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L37" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="M37" s="5">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="N37" s="5">
-        <v>35</v>
-      </c>
-      <c r="O37" s="5">
-        <v>35</v>
-      </c>
-      <c r="P37" s="5">
-        <v>35</v>
-      </c>
-      <c r="Q37" s="5">
-        <v>35</v>
-      </c>
-      <c r="R37" s="5">
-        <v>35</v>
-      </c>
-      <c r="S37" s="5">
-        <v>35</v>
-      </c>
-      <c r="T37" s="5">
-        <v>35</v>
-      </c>
-      <c r="U37" s="5">
-        <v>35</v>
-      </c>
-      <c r="V37" s="5">
-        <v>35</v>
-      </c>
-      <c r="W37" s="5">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="O37" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P37" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q37" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R37" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="S37" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="T37" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="U37" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="V37" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="W37" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="X37" s="5">
         <v>35</v>
       </c>
-      <c r="Y37" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z37" s="5">
-        <v>35</v>
-      </c>
-      <c r="AA37" s="5">
-        <v>35</v>
+      <c r="Y37" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z37" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA37" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="38" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B38" s="5">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C38" s="5">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D38" s="5">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E38" s="5">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F38" s="5">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G38" s="5">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H38" s="5">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I38" s="5">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J38" s="5">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K38" s="5">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L38" s="5">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M38" s="5">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N38" s="5">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O38" s="5">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P38" s="5">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Q38" s="5">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="R38" s="5">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S38" s="5">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="T38" s="5">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="U38" s="5">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="V38" s="5">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="W38" s="5">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X38" s="5">
-        <v>36</v>
-      </c>
-      <c r="Y38" s="5">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="Y38" s="7">
+        <v>0</v>
       </c>
       <c r="Z38" s="5">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AA38" s="5">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39" s="5">
         <v>36</v>
@@ -3764,20 +3773,103 @@
         <v>36</v>
       </c>
       <c r="X39" s="5">
+        <v>36</v>
+      </c>
+      <c r="Y39" s="5">
+        <v>36</v>
+      </c>
+      <c r="Z39" s="5">
+        <v>36</v>
+      </c>
+      <c r="AA39" s="5">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
+        <v>37</v>
+      </c>
+      <c r="B40" s="5">
+        <v>36</v>
+      </c>
+      <c r="C40" s="5">
+        <v>36</v>
+      </c>
+      <c r="D40" s="5">
+        <v>36</v>
+      </c>
+      <c r="E40" s="5">
+        <v>36</v>
+      </c>
+      <c r="F40" s="5">
+        <v>36</v>
+      </c>
+      <c r="G40" s="5">
+        <v>36</v>
+      </c>
+      <c r="H40" s="5">
+        <v>36</v>
+      </c>
+      <c r="I40" s="5">
+        <v>36</v>
+      </c>
+      <c r="J40" s="5">
+        <v>36</v>
+      </c>
+      <c r="K40" s="5">
+        <v>36</v>
+      </c>
+      <c r="L40" s="5">
+        <v>36</v>
+      </c>
+      <c r="M40" s="5">
+        <v>36</v>
+      </c>
+      <c r="N40" s="5">
+        <v>37</v>
+      </c>
+      <c r="O40" s="5">
+        <v>36</v>
+      </c>
+      <c r="P40" s="5">
+        <v>36</v>
+      </c>
+      <c r="Q40" s="5">
+        <v>36</v>
+      </c>
+      <c r="R40" s="5">
+        <v>36</v>
+      </c>
+      <c r="S40" s="5">
+        <v>36</v>
+      </c>
+      <c r="T40" s="5">
+        <v>36</v>
+      </c>
+      <c r="U40" s="5">
+        <v>36</v>
+      </c>
+      <c r="V40" s="5">
+        <v>36</v>
+      </c>
+      <c r="W40" s="5">
+        <v>36</v>
+      </c>
+      <c r="X40" s="5">
         <v>0</v>
       </c>
-      <c r="Y39" s="5">
-        <v>36</v>
-      </c>
-      <c r="Z39" s="5">
-        <v>36</v>
-      </c>
-      <c r="AA39" s="5">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="D43" t="s">
+      <c r="Y40" s="5">
+        <v>36</v>
+      </c>
+      <c r="Z40" s="5">
+        <v>36</v>
+      </c>
+      <c r="AA40" s="5">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="44" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="D44" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>